<commit_message>
Added master table to excel.  Added gains table to the doc
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruggler\Desktop\project214\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="19155" windowHeight="7740"/>
+    <workbookView xWindow="1410" yWindow="75" windowWidth="19155" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
   <si>
     <t>node</t>
   </si>
@@ -163,12 +168,150 @@
     <t>gm in scale of 0.001; from CG vs cascode equation
 CG gain ~ 1000 bigger than cascode</t>
   </si>
+  <si>
+    <t>Vov</t>
+  </si>
+  <si>
+    <t>W/L</t>
+  </si>
+  <si>
+    <t>gm</t>
+  </si>
+  <si>
+    <t>R1 = 6250, R2 = 25000</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Gain</t>
+  </si>
+  <si>
+    <t>Bandwidth</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>gm2</t>
+  </si>
+  <si>
+    <t>gm4</t>
+  </si>
+  <si>
+    <t>gm7</t>
+  </si>
+  <si>
+    <t>gm8</t>
+  </si>
+  <si>
+    <t>gm10</t>
+  </si>
+  <si>
+    <t>Looking at reasonable ranges for any gm</t>
+  </si>
+  <si>
+    <t>Spreadsheet for calculating outputs given inputs</t>
+  </si>
+  <si>
+    <t>Cgs2</t>
+  </si>
+  <si>
+    <t>Cgs4</t>
+  </si>
+  <si>
+    <t>Cgs7</t>
+  </si>
+  <si>
+    <t>Cgs8</t>
+  </si>
+  <si>
+    <t>Cgs10</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Rules</t>
+  </si>
+  <si>
+    <t>R2/R1 &lt; 4</t>
+  </si>
+  <si>
+    <t>R3/R4 &lt; 4</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Dependent Variables</t>
+  </si>
+  <si>
+    <t>WL2</t>
+  </si>
+  <si>
+    <t>WL4</t>
+  </si>
+  <si>
+    <t>WL7</t>
+  </si>
+  <si>
+    <t>WL8</t>
+  </si>
+  <si>
+    <t>Looking at reasonable ranges for any Cgs</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>TC1</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
+    <t>TC4</t>
+  </si>
+  <si>
+    <t>TC1 %</t>
+  </si>
+  <si>
+    <t>TC2 %</t>
+  </si>
+  <si>
+    <t>TC3 %</t>
+  </si>
+  <si>
+    <t>TC4 %</t>
+  </si>
+  <si>
+    <t>TC5</t>
+  </si>
+  <si>
+    <t>TC5 %</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +326,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -192,10 +343,168 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="15">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -204,20 +513,361 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="42">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -266,7 +916,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -301,7 +951,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -510,16 +1160,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="31.42578125" customWidth="1"/>
     <col min="5" max="5" width="30.5703125" customWidth="1"/>
@@ -671,6 +1321,9 @@
       <c r="E11" t="s">
         <v>34</v>
       </c>
+      <c r="F11" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -714,9 +1367,688 @@
         <v>37</v>
       </c>
     </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="E20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="C21" s="2">
+        <v>4</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="2">
+        <v>2</v>
+      </c>
+      <c r="G21" s="2">
+        <f>15*G22</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="2">
+        <f>1/15</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="C22" s="2">
+        <v>15</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="2">
+        <v>2</v>
+      </c>
+      <c r="G22" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="12">
+        <f>B21*B22*0.00005</f>
+        <v>5.0000000000000008E-7</v>
+      </c>
+      <c r="C23" s="12">
+        <f>C21*C22*0.00005</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="2">
+        <f>F21*F22*2/3*0.0000000000000023</f>
+        <v>6.1333333333333325E-15</v>
+      </c>
+      <c r="G23" s="2">
+        <f>G21*G22*2/3*0.0000000000000023</f>
+        <v>2.2999999999999999E-12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="10">
+        <f>(B39*B40/(B39+B40))   *   (-B44*B41*B42/(B41+B42))   *   (-B45/B46)   *   (B47*20000/(B47*20000 + 1))</f>
+        <v>45878.816642936239</v>
+      </c>
+      <c r="C28" s="10">
+        <f t="shared" ref="C28:F28" si="1">(C39*C40/(C39+C40))   *   (-C44*C41*C42/(C41+C42))   *   (-C45/C46)   *   (C47*20000/(C47*20000 + 1))</f>
+        <v>33134.700908787287</v>
+      </c>
+      <c r="D28" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E28" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F28" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="14">
+        <f>1/(SUM(B58:B62) * 2 * 3.14159)</f>
+        <v>17855332.42198291</v>
+      </c>
+      <c r="C29" s="14">
+        <f t="shared" ref="C29:F29" si="2">1/(2*3.14159)*1/(   (0.00000000000022 + C48)/C43   +   (C39*C40*C49/(C39+C40))   +   (C41*C42*C50)/(C41+C42)   +   (C51+C52*(1+C47*20000))/C46   +   20000*(0.00000000000025+C52*(1+1/(20000*C47)))/(1+20000*C47))</f>
+        <v>111088058.04342037</v>
+      </c>
+      <c r="D29" s="14" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E29" s="14" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F29" s="11" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="27"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="10">
+        <f>IF(B40/B39&lt;=4, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="C32" s="10">
+        <f t="shared" ref="C32:F32" si="3">IF(C40/C39&lt;=4, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D32" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E32" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F32" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="10">
+        <f>IF(B41/B42&lt;=4, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="C33" s="10">
+        <f t="shared" ref="C33:F33" si="4">IF(C41/C42&lt;=4, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D33" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E33" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F33" s="8" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="20"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="20"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="8"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="20"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="8"/>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="21"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="29"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="10">
+        <v>10000</v>
+      </c>
+      <c r="C39" s="10">
+        <v>6500</v>
+      </c>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="8"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="10">
+        <v>25000</v>
+      </c>
+      <c r="C40" s="10">
+        <v>25000</v>
+      </c>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="8"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="10">
+        <v>25000</v>
+      </c>
+      <c r="C41" s="10">
+        <v>25000</v>
+      </c>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="8"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="10">
+        <v>7250</v>
+      </c>
+      <c r="C42" s="10">
+        <v>7250</v>
+      </c>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="8"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="C43" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="8"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="C44" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="8"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="10">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="C45" s="10">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="C46" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="8"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="C47" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="8"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" s="10">
+        <v>2.2999999999999998E-13</v>
+      </c>
+      <c r="C48" s="10">
+        <v>6.0999999999999997E-15</v>
+      </c>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="8"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="16">
+        <v>2.2999999999999998E-13</v>
+      </c>
+      <c r="C49" s="16">
+        <v>6.0999999999999997E-15</v>
+      </c>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="8"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="16">
+        <v>2.2999999999999998E-13</v>
+      </c>
+      <c r="C50" s="16">
+        <v>6.1000000000000005E-14</v>
+      </c>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="8"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" s="16">
+        <v>2.2999999999999998E-13</v>
+      </c>
+      <c r="C51" s="16">
+        <v>4.5999999999999996E-13</v>
+      </c>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="8"/>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="17">
+        <v>2.2999999999999998E-13</v>
+      </c>
+      <c r="C52" s="17">
+        <v>6.0999999999999997E-15</v>
+      </c>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="9"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" s="29"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="7"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="10">
+        <f>B48*3/2/0.0000000000000023</f>
+        <v>149.99999999999997</v>
+      </c>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="8"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" s="10">
+        <f t="shared" ref="B55:B58" si="5">B49*3/2/0.0000000000000023</f>
+        <v>149.99999999999997</v>
+      </c>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="8"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" s="10">
+        <f t="shared" si="5"/>
+        <v>149.99999999999997</v>
+      </c>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="8"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" s="10">
+        <f t="shared" si="5"/>
+        <v>149.99999999999997</v>
+      </c>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="8"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58" s="25">
+        <f>(0.00000000000022 + B48)/B43</f>
+        <v>4.5E-10</v>
+      </c>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="8"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B59" s="25">
+        <f>(B39*B40*B49/(B39+B40))</f>
+        <v>1.6428571428571428E-9</v>
+      </c>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="8"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" s="10">
+        <f>(B41*B42*B50)/(B41+B42)</f>
+        <v>1.2926356589147286E-9</v>
+      </c>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="8"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B61" s="10">
+        <f>(B51+B52*(1+B47*20000))/B46</f>
+        <v>5.0599999999999987E-9</v>
+      </c>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="8"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B62" s="10">
+        <f xml:space="preserve"> 20000*(0.00000000000025+B52*(1+1/(20000*B47)))/(1+20000*B47)</f>
+        <v>4.6809523809523803E-10</v>
+      </c>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="8"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B63" s="32">
+        <f>B58/SUM(B$58:B$62)</f>
+        <v>5.0484720405219563E-2</v>
+      </c>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="8"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="B64" s="32">
+        <f t="shared" ref="B64:B67" si="6">B59/SUM(B$58:B$62)</f>
+        <v>0.18430929671746824</v>
+      </c>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="8"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B65" s="32">
+        <f t="shared" si="6"/>
+        <v>0.14501855516917075</v>
+      </c>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="8"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B66" s="32">
+        <f t="shared" si="6"/>
+        <v>0.56767263388980205</v>
+      </c>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="8"/>
+    </row>
+    <row r="67" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B67" s="34">
+        <f t="shared" si="6"/>
+        <v>5.2514793818339497E-2</v>
+      </c>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="9"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A26:C26"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B28:F28">
+    <cfRule type="expression" dxfId="11" priority="6">
+      <formula>B28&gt;30000</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="5">
+      <formula>B28&lt;30000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29:F29">
+    <cfRule type="expression" dxfId="9" priority="4">
+      <formula>B29&gt;90000000</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="3">
+      <formula>B29&lt;90000000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30:F30">
+    <cfRule type="expression" dxfId="7" priority="2">
+      <formula>B30&lt;0.002</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>B30&gt;0.002</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added gm over id tab
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruggler\Desktop\project214\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="75" windowWidth="19155" windowHeight="7740"/>
+    <workbookView xWindow="1410" yWindow="75" windowWidth="19155" windowHeight="7740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="gmid" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="114">
   <si>
     <t>node</t>
   </si>
@@ -305,6 +300,93 @@
   </si>
   <si>
     <t>TC5 %</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>gm/id</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Vgs</t>
+  </si>
+  <si>
+    <t>Vt</t>
+  </si>
+  <si>
+    <t>kp_n</t>
+  </si>
+  <si>
+    <t>M10</t>
+  </si>
+  <si>
+    <t>MP8</t>
+  </si>
+  <si>
+    <t>ids</t>
+  </si>
+  <si>
+    <t>tau</t>
+  </si>
+  <si>
+    <t>gain allocated</t>
+  </si>
+  <si>
+    <t>tau allocated</t>
+  </si>
+  <si>
+    <t>MN1</t>
+  </si>
+  <si>
+    <t>MN2</t>
+  </si>
+  <si>
+    <t>Cin</t>
+  </si>
+  <si>
+    <t>xtor</t>
+  </si>
+  <si>
+    <t>MP3</t>
+  </si>
+  <si>
+    <t>MP4</t>
+  </si>
+  <si>
+    <t>MN6</t>
+  </si>
+  <si>
+    <t>MP5</t>
+  </si>
+  <si>
+    <t>I total</t>
+  </si>
+  <si>
+    <t>I R</t>
+  </si>
+  <si>
+    <t>I xtor</t>
+  </si>
+  <si>
+    <t>vdd</t>
+  </si>
+  <si>
+    <t>MN7</t>
+  </si>
+  <si>
+    <t>MN9</t>
+  </si>
+  <si>
+    <t>vbias_n</t>
+  </si>
+  <si>
+    <t>vbias_p</t>
   </si>
 </sst>
 </file>
@@ -513,16 +595,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -561,18 +639,16 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -612,251 +688,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -916,7 +747,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -951,7 +782,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1162,7 +993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -1368,16 +1199,16 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="5"/>
-      <c r="E20" s="3" t="s">
+      <c r="B20" s="33"/>
+      <c r="C20" s="34"/>
+      <c r="E20" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="5"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="34"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -1422,14 +1253,14 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="8">
         <f>B21*B22*0.00005</f>
         <v>5.0000000000000008E-7</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="8">
         <f>C21*C22*0.00005</f>
         <v>3.0000000000000001E-3</v>
       </c>
@@ -1446,576 +1277,576 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="7"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="6">
         <f>(B39*B40/(B39+B40))   *   (-B44*B41*B42/(B41+B42))   *   (-B45/B46)   *   (B47*20000/(B47*20000 + 1))</f>
         <v>45878.816642936239</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="6">
         <f t="shared" ref="C28:F28" si="1">(C39*C40/(C39+C40))   *   (-C44*C41*C42/(C41+C42))   *   (-C45/C46)   *   (C47*20000/(C47*20000 + 1))</f>
         <v>33134.700908787287</v>
       </c>
-      <c r="D28" s="10" t="e">
+      <c r="D28" s="6" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E28" s="10" t="e">
+      <c r="E28" s="6" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F28" s="8" t="e">
+      <c r="F28" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B29" s="10">
         <f>1/(SUM(B58:B62) * 2 * 3.14159)</f>
         <v>17855332.42198291</v>
       </c>
-      <c r="C29" s="14">
+      <c r="C29" s="10">
         <f t="shared" ref="C29:F29" si="2">1/(2*3.14159)*1/(   (0.00000000000022 + C48)/C43   +   (C39*C40*C49/(C39+C40))   +   (C41*C42*C50)/(C41+C42)   +   (C51+C52*(1+C47*20000))/C46   +   20000*(0.00000000000025+C52*(1+1/(20000*C47)))/(1+20000*C47))</f>
         <v>111088058.04342037</v>
       </c>
-      <c r="D29" s="14" t="e">
+      <c r="D29" s="10" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E29" s="14" t="e">
+      <c r="E29" s="10" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F29" s="11" t="e">
+      <c r="F29" s="7" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="9"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="7"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="6">
         <f>IF(B40/B39&lt;=4, 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="6">
         <f t="shared" ref="C32:F32" si="3">IF(C40/C39&lt;=4, 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="D32" s="10" t="e">
+      <c r="D32" s="6" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E32" s="10" t="e">
+      <c r="E32" s="6" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F32" s="8" t="e">
+      <c r="F32" s="4" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="6">
         <f>IF(B41/B42&lt;=4, 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="6">
         <f t="shared" ref="C33:F33" si="4">IF(C41/C42&lt;=4, 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="D33" s="10" t="e">
+      <c r="D33" s="6" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E33" s="10" t="e">
+      <c r="E33" s="6" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F33" s="8" t="e">
+      <c r="F33" s="4" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="8"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="8"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="8"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="21"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="9"/>
+      <c r="A37" s="17"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="29"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="7"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="3"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="22" t="s">
+      <c r="A39" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="10">
+      <c r="B39" s="6">
         <v>10000</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="6">
         <v>6500</v>
       </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="8"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="4"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="22" t="s">
+      <c r="A40" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="10">
+      <c r="B40" s="6">
         <v>25000</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="6">
         <v>25000</v>
       </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="8"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="22" t="s">
+      <c r="A41" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="10">
+      <c r="B41" s="6">
         <v>25000</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C41" s="6">
         <v>25000</v>
       </c>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="8"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="10">
+      <c r="B42" s="6">
         <v>7250</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C42" s="6">
         <v>7250</v>
       </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="8"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B43" s="10">
+      <c r="B43" s="6">
         <v>1E-3</v>
       </c>
-      <c r="C43" s="10">
+      <c r="C43" s="6">
         <v>1E-3</v>
       </c>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="8"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="22" t="s">
+      <c r="A44" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="10">
+      <c r="B44" s="6">
         <v>1E-3</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="6">
         <v>1E-3</v>
       </c>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="8"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="10">
+      <c r="B45" s="6">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C45" s="6">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="8"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="10">
+      <c r="B46" s="6">
         <v>1E-3</v>
       </c>
-      <c r="C46" s="10">
+      <c r="C46" s="6">
         <v>1E-3</v>
       </c>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="8"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="22" t="s">
+      <c r="A47" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="10">
+      <c r="B47" s="6">
         <v>1E-3</v>
       </c>
-      <c r="C47" s="10">
+      <c r="C47" s="6">
         <v>1E-3</v>
       </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="8"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="4"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="22" t="s">
+      <c r="A48" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="10">
+      <c r="B48" s="6">
         <v>2.2999999999999998E-13</v>
       </c>
-      <c r="C48" s="10">
+      <c r="C48" s="6">
         <v>6.0999999999999997E-15</v>
       </c>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="8"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="4"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="22" t="s">
+      <c r="A49" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="16">
+      <c r="B49" s="12">
         <v>2.2999999999999998E-13</v>
       </c>
-      <c r="C49" s="16">
+      <c r="C49" s="12">
         <v>6.0999999999999997E-15</v>
       </c>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="8"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="4"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="22" t="s">
+      <c r="A50" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="B50" s="16">
+      <c r="B50" s="12">
         <v>2.2999999999999998E-13</v>
       </c>
-      <c r="C50" s="16">
+      <c r="C50" s="12">
         <v>6.1000000000000005E-14</v>
       </c>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="8"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="4"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="22" t="s">
+      <c r="A51" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B51" s="16">
+      <c r="B51" s="12">
         <v>2.2999999999999998E-13</v>
       </c>
-      <c r="C51" s="16">
+      <c r="C51" s="12">
         <v>4.5999999999999996E-13</v>
       </c>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="8"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="4"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="23" t="s">
+      <c r="A52" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B52" s="17">
+      <c r="B52" s="13">
         <v>2.2999999999999998E-13</v>
       </c>
-      <c r="C52" s="17">
+      <c r="C52" s="13">
         <v>6.0999999999999997E-15</v>
       </c>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="9"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="5"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="31" t="s">
+      <c r="A53" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="B53" s="29"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="7"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="3"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="22" t="s">
+      <c r="A54" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="B54" s="10">
+      <c r="B54" s="6">
         <f>B48*3/2/0.0000000000000023</f>
         <v>149.99999999999997</v>
       </c>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="8"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="4"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="22" t="s">
+      <c r="A55" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="10">
-        <f t="shared" ref="B55:B58" si="5">B49*3/2/0.0000000000000023</f>
+      <c r="B55" s="6">
+        <f t="shared" ref="B55:B57" si="5">B49*3/2/0.0000000000000023</f>
         <v>149.99999999999997</v>
       </c>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="8"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="4"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="22" t="s">
+      <c r="A56" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B56" s="10">
+      <c r="B56" s="6">
         <f t="shared" si="5"/>
         <v>149.99999999999997</v>
       </c>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="8"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="4"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="22" t="s">
+      <c r="A57" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B57" s="10">
+      <c r="B57" s="6">
         <f t="shared" si="5"/>
         <v>149.99999999999997</v>
       </c>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="8"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="4"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="24" t="s">
+      <c r="A58" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="B58" s="25">
+      <c r="B58" s="21">
         <f>(0.00000000000022 + B48)/B43</f>
         <v>4.5E-10</v>
       </c>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="8"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="4"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="24" t="s">
+      <c r="A59" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="B59" s="25">
+      <c r="B59" s="21">
         <f>(B39*B40*B49/(B39+B40))</f>
         <v>1.6428571428571428E-9</v>
       </c>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="8"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="4"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="24" t="s">
+      <c r="A60" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B60" s="10">
+      <c r="B60" s="6">
         <f>(B41*B42*B50)/(B41+B42)</f>
         <v>1.2926356589147286E-9</v>
       </c>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="8"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="4"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="24" t="s">
+      <c r="A61" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B61" s="10">
+      <c r="B61" s="6">
         <f>(B51+B52*(1+B47*20000))/B46</f>
         <v>5.0599999999999987E-9</v>
       </c>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="8"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="4"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="24" t="s">
+      <c r="A62" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B62" s="10">
+      <c r="B62" s="6">
         <f xml:space="preserve"> 20000*(0.00000000000025+B52*(1+1/(20000*B47)))/(1+20000*B47)</f>
         <v>4.6809523809523803E-10</v>
       </c>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="8"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="4"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="24" t="s">
+      <c r="A63" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="B63" s="32">
+      <c r="B63" s="28">
         <f>B58/SUM(B$58:B$62)</f>
         <v>5.0484720405219563E-2</v>
       </c>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="8"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="4"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="24" t="s">
+      <c r="A64" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B64" s="32">
+      <c r="B64" s="28">
         <f t="shared" ref="B64:B67" si="6">B59/SUM(B$58:B$62)</f>
         <v>0.18430929671746824</v>
       </c>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="8"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="4"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="24" t="s">
+      <c r="A65" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B65" s="32">
+      <c r="B65" s="28">
         <f t="shared" si="6"/>
         <v>0.14501855516917075</v>
       </c>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-      <c r="E65" s="10"/>
-      <c r="F65" s="8"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="4"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="24" t="s">
+      <c r="A66" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="B66" s="32">
+      <c r="B66" s="28">
         <f t="shared" si="6"/>
         <v>0.56767263388980205</v>
       </c>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-      <c r="E66" s="10"/>
-      <c r="F66" s="8"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="4"/>
     </row>
     <row r="67" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="33" t="s">
+      <c r="A67" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="B67" s="34">
+      <c r="B67" s="30">
         <f t="shared" si="6"/>
         <v>5.2514793818339497E-2</v>
       </c>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="15"/>
-      <c r="F67" s="9"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2024,27 +1855,27 @@
     <mergeCell ref="A26:C26"/>
   </mergeCells>
   <conditionalFormatting sqref="B28:F28">
-    <cfRule type="expression" dxfId="11" priority="6">
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>B28&lt;30000</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>B28&gt;30000</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="5">
-      <formula>B28&lt;30000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:F29">
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>B29&lt;90000000</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>B29&gt;90000000</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="3">
-      <formula>B29&lt;90000000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:F30">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>B30&gt;0.002</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>B30&lt;0.002</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="1">
-      <formula>B30&gt;0.002</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2054,24 +1885,466 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M1" t="s">
+        <v>101</v>
+      </c>
+      <c r="N1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O1" t="s">
+        <v>97</v>
+      </c>
+      <c r="P1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>106</v>
+      </c>
+      <c r="R1" t="s">
+        <v>107</v>
+      </c>
+      <c r="S1" t="s">
+        <v>108</v>
+      </c>
+      <c r="T1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.5</v>
+      </c>
+      <c r="B2" s="31">
+        <v>2.4999999999999999E-13</v>
+      </c>
+      <c r="C2" s="31">
+        <v>110000000</v>
+      </c>
+      <c r="D2" s="31">
+        <f>1/(2*3.1415*C2)</f>
+        <v>1.4469057919638852E-9</v>
+      </c>
+      <c r="E2" s="31">
+        <f>B2/D2</f>
+        <v>1.7278249999999999E-4</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2" s="31">
+        <f>E2/F2</f>
+        <v>1.727825E-5</v>
+      </c>
+      <c r="H2" s="31">
+        <f>(2*G2)/E2</f>
+        <v>0.2</v>
+      </c>
+      <c r="I2" s="31">
+        <f>H2+A2</f>
+        <v>0.7</v>
+      </c>
+      <c r="J2" s="31">
+        <f>(2*G2*K2)/(L2*H2*H2)</f>
+        <v>1.7278249999999997E-5</v>
+      </c>
+      <c r="K2" s="31">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="L2" s="31">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="M2" t="s">
+        <v>92</v>
+      </c>
+      <c r="P2" s="31">
+        <v>2.2E-13</v>
+      </c>
+      <c r="Q2" s="31">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="R2" s="31">
+        <f>0.3*Q2</f>
+        <v>1.2E-4</v>
+      </c>
+      <c r="S2" s="31">
+        <f>Q2-R2</f>
+        <v>2.8000000000000003E-4</v>
+      </c>
+      <c r="T2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E3" s="31"/>
+      <c r="G3" s="31">
+        <f>G2</f>
+        <v>1.727825E-5</v>
+      </c>
+      <c r="H3" s="31">
+        <f>SQRT((2*G3)/L3*(J3/K3))</f>
+        <v>0.83134228811001787</v>
+      </c>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="K3" s="31">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="L3" s="31">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="M3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E5" s="31">
+        <f>P2*O5</f>
+        <v>1.21E-4</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5" s="31">
+        <f>E5/F5</f>
+        <v>1.2099999999999999E-5</v>
+      </c>
+      <c r="H5" s="31">
+        <f>(2*G5)/E5</f>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="J5" s="31">
+        <f>(2*G5*K5)/(L5*H5*H5)</f>
+        <v>1.2100000000000003E-5</v>
+      </c>
+      <c r="K5" s="31">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="L5" s="31">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="M5" t="s">
+        <v>99</v>
+      </c>
+      <c r="O5" s="31">
+        <f>C2/0.2</f>
+        <v>550000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G6" s="31">
+        <f>G5</f>
+        <v>1.2099999999999999E-5</v>
+      </c>
+      <c r="H6" s="31">
+        <f>H3</f>
+        <v>0.83134228811001787</v>
+      </c>
+      <c r="J6" s="31">
+        <f>(2*G6*K6)/(L6*H6*H6)</f>
+        <v>2.1009072099315612E-6</v>
+      </c>
+      <c r="K6" s="31">
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="L6" s="31">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="M6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G7" s="31">
+        <f>G5</f>
+        <v>1.2099999999999999E-5</v>
+      </c>
+      <c r="H7" s="31">
+        <f>SQRT((2*G7)/L7*(J7/K7))</f>
+        <v>1.3914021704740869</v>
+      </c>
+      <c r="J7" s="31">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="K7" s="31">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="L7" s="31">
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="M7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G8" s="31">
+        <f>0.5*L8*(J8/K8)*H8*H8</f>
+        <v>1.727825E-5</v>
+      </c>
+      <c r="H8" s="31">
+        <f>H3</f>
+        <v>0.83134228811001787</v>
+      </c>
+      <c r="J8" s="31">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="K8" s="31">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="L8" s="31">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="M8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E9" s="31">
+        <f>F9*G9</f>
+        <v>1.7278249999999999E-4</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9" s="31">
+        <f>G8</f>
+        <v>1.727825E-5</v>
+      </c>
+      <c r="H9" s="31">
+        <f>(2*G9)/E9</f>
+        <v>0.2</v>
+      </c>
+      <c r="J9" s="31">
+        <f>(2*G9*K9)/(L9*H9*H9)</f>
+        <v>3.4556499999999993E-5</v>
+      </c>
+      <c r="K9" s="31">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="L9" s="31">
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="M9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E10" s="31">
+        <f>E9</f>
+        <v>1.7278249999999999E-4</v>
+      </c>
+      <c r="G10" s="31">
+        <f>G9</f>
+        <v>1.727825E-5</v>
+      </c>
+      <c r="H10" s="31">
+        <f>(2*G10)/E10</f>
+        <v>0.2</v>
+      </c>
+      <c r="J10" s="31">
+        <f>(2*G10*K10)/(L10*H10*H10)</f>
+        <v>3.4556499999999993E-5</v>
+      </c>
+      <c r="K10" s="31">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="L10" s="31">
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="M10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G11" s="31">
+        <f>S2-G2-G9-G7</f>
+        <v>2.3334350000000004E-4</v>
+      </c>
+      <c r="H11" s="31">
+        <f>T2-I2-A2</f>
+        <v>1.3</v>
+      </c>
+      <c r="J11" s="31">
+        <f>(2*G11*K11)/(L11*H11*H11)</f>
+        <v>1.1045846153846153E-5</v>
+      </c>
+      <c r="K11" s="31">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="L11" s="31">
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="M11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E12" s="31">
+        <f>F12*G12</f>
+        <v>2.3334350000000005E-3</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12" s="31">
+        <f>G11</f>
+        <v>2.3334350000000004E-4</v>
+      </c>
+      <c r="H12" s="31">
+        <f>(2*G12)/E12</f>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="J12" s="31">
+        <f>(2*G12*K12)/(L12*H12*H12)</f>
+        <v>2.3334350000000009E-4</v>
+      </c>
+      <c r="K12" s="31">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="L12" s="31">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="M12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="31">
+        <f>2.5-A2 - H7</f>
+        <v>0.60859782952591313</v>
+      </c>
+      <c r="B20" s="31">
+        <f>-2.5+H6+A2</f>
+        <v>-1.1686577118899821</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="31">
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="31">
+        <v>2.1999999999999999E-5</v>
+      </c>
+      <c r="D2" s="31">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="E2" s="31">
+        <f>0.5*A2*(C2/D2)*F2</f>
+        <v>9.6937500000000005E-5</v>
+      </c>
+      <c r="F2" s="31">
+        <v>0.70499999999999996</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
beefed up gm over id data to match our CP2 spice netlist result
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="75" windowWidth="19155" windowHeight="7740" activeTab="1"/>
+    <workbookView xWindow="1410" yWindow="75" windowWidth="19155" windowHeight="7740" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="gmid" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="156">
   <si>
     <t>node</t>
   </si>
@@ -387,6 +388,132 @@
   </si>
   <si>
     <t>vbias_p</t>
+  </si>
+  <si>
+    <t>power target</t>
+  </si>
+  <si>
+    <t>R power</t>
+  </si>
+  <si>
+    <t>Vdd</t>
+  </si>
+  <si>
+    <t>Vss</t>
+  </si>
+  <si>
+    <t>xtor power</t>
+  </si>
+  <si>
+    <t>Ids_total</t>
+  </si>
+  <si>
+    <t>Ids_stack1</t>
+  </si>
+  <si>
+    <t>Ids_stack2</t>
+  </si>
+  <si>
+    <t>Ids_stack3</t>
+  </si>
+  <si>
+    <t>Ids_stack4</t>
+  </si>
+  <si>
+    <t>Ids_sum</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>M4</t>
+  </si>
+  <si>
+    <t>M5</t>
+  </si>
+  <si>
+    <t>M6</t>
+  </si>
+  <si>
+    <t>M7</t>
+  </si>
+  <si>
+    <t>M8</t>
+  </si>
+  <si>
+    <t>M9</t>
+  </si>
+  <si>
+    <t>spice Vov</t>
+  </si>
+  <si>
+    <t>stack1</t>
+  </si>
+  <si>
+    <t>stack2</t>
+  </si>
+  <si>
+    <t>stack3</t>
+  </si>
+  <si>
+    <t>stack4</t>
+  </si>
+  <si>
+    <t>Ids %</t>
+  </si>
+  <si>
+    <t>spice Ids</t>
+  </si>
+  <si>
+    <t>spice Ids%</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>spice BW</t>
+  </si>
+  <si>
+    <t>Spice gain in db</t>
+  </si>
+  <si>
+    <t>spice gain in ohms</t>
+  </si>
+  <si>
+    <t>spice gm</t>
+  </si>
+  <si>
+    <t>calc Vov</t>
+  </si>
+  <si>
+    <t>% error</t>
+  </si>
+  <si>
+    <t>calc gm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ids </t>
+  </si>
+  <si>
+    <t>Ids allocated</t>
+  </si>
+  <si>
+    <t>spice W</t>
+  </si>
+  <si>
+    <t>calc W</t>
+  </si>
+  <si>
+    <t>spice L</t>
+  </si>
+  <si>
+    <t>calc L</t>
   </si>
 </sst>
 </file>
@@ -417,12 +544,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="15">
@@ -595,7 +740,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -644,6 +789,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1887,8 +2038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1982,23 +2133,23 @@
         <v>1.7278249999999999E-4</v>
       </c>
       <c r="F2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G2" s="31">
         <f>E2/F2</f>
-        <v>1.727825E-5</v>
+        <v>2.1597812499999999E-5</v>
       </c>
       <c r="H2" s="31">
         <f>(2*G2)/E2</f>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="I2" s="31">
         <f>H2+A2</f>
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="J2" s="31">
         <f>(2*G2*K2)/(L2*H2*H2)</f>
-        <v>1.7278249999999997E-5</v>
+        <v>1.3822599999999999E-5</v>
       </c>
       <c r="K2" s="31">
         <v>9.9999999999999995E-7</v>
@@ -2031,11 +2182,11 @@
       <c r="E3" s="31"/>
       <c r="G3" s="31">
         <f>G2</f>
-        <v>1.727825E-5</v>
+        <v>2.1597812499999999E-5</v>
       </c>
       <c r="H3" s="31">
         <f>SQRT((2*G3)/L3*(J3/K3))</f>
-        <v>0.83134228811001787</v>
+        <v>0.92946893439210754</v>
       </c>
       <c r="I3" s="31"/>
       <c r="J3" s="31">
@@ -2062,22 +2213,22 @@
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E5" s="31">
         <f>P2*O5</f>
-        <v>1.21E-4</v>
+        <v>4.0333333333333334E-4</v>
       </c>
       <c r="F5">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G5" s="31">
         <f>E5/F5</f>
-        <v>1.2099999999999999E-5</v>
+        <v>1.3444444444444444E-4</v>
       </c>
       <c r="H5" s="31">
         <f>(2*G5)/E5</f>
-        <v>0.19999999999999998</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J5" s="31">
         <f>(2*G5*K5)/(L5*H5*H5)</f>
-        <v>1.2100000000000003E-5</v>
+        <v>1.2099999999999999E-5</v>
       </c>
       <c r="K5" s="31">
         <v>9.9999999999999995E-7</v>
@@ -2089,22 +2240,22 @@
         <v>99</v>
       </c>
       <c r="O5" s="31">
-        <f>C2/0.2</f>
-        <v>550000000</v>
+        <f>C2/0.06</f>
+        <v>1833333333.3333335</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G6" s="31">
         <f>G5</f>
-        <v>1.2099999999999999E-5</v>
+        <v>1.3444444444444444E-4</v>
       </c>
       <c r="H6" s="31">
         <f>H3</f>
-        <v>0.83134228811001787</v>
+        <v>0.92946893439210754</v>
       </c>
       <c r="J6" s="31">
         <f>(2*G6*K6)/(L6*H6*H6)</f>
-        <v>2.1009072099315612E-6</v>
+        <v>1.8674730754947213E-5</v>
       </c>
       <c r="K6" s="31">
         <v>3.0000000000000001E-6</v>
@@ -2119,11 +2270,11 @@
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G7" s="31">
         <f>G5</f>
-        <v>1.2099999999999999E-5</v>
+        <v>1.3444444444444444E-4</v>
       </c>
       <c r="H7" s="31">
         <f>SQRT((2*G7)/L7*(J7/K7))</f>
-        <v>1.3914021704740869</v>
+        <v>4.6380072349136228</v>
       </c>
       <c r="J7" s="31">
         <v>1.9999999999999999E-6</v>
@@ -2141,14 +2292,14 @@
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G8" s="31">
         <f>0.5*L8*(J8/K8)*H8*H8</f>
-        <v>1.727825E-5</v>
+        <v>6.4793437500000001E-5</v>
       </c>
       <c r="H8" s="31">
         <f>H3</f>
-        <v>0.83134228811001787</v>
+        <v>0.92946893439210754</v>
       </c>
       <c r="J8" s="31">
-        <v>1.9999999999999999E-6</v>
+        <v>6.0000000000000002E-6</v>
       </c>
       <c r="K8" s="31">
         <v>1.9999999999999999E-6</v>
@@ -2163,22 +2314,22 @@
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E9" s="31">
         <f>F9*G9</f>
-        <v>1.7278249999999999E-4</v>
+        <v>3.2396718749999999E-4</v>
       </c>
       <c r="F9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G9" s="31">
         <f>G8</f>
-        <v>1.727825E-5</v>
+        <v>6.4793437500000001E-5</v>
       </c>
       <c r="H9" s="31">
         <f>(2*G9)/E9</f>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="J9" s="31">
         <f>(2*G9*K9)/(L9*H9*H9)</f>
-        <v>3.4556499999999993E-5</v>
+        <v>3.2396718749999994E-5</v>
       </c>
       <c r="K9" s="31">
         <v>9.9999999999999995E-7</v>
@@ -2193,19 +2344,19 @@
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E10" s="31">
         <f>E9</f>
-        <v>1.7278249999999999E-4</v>
+        <v>3.2396718749999999E-4</v>
       </c>
       <c r="G10" s="31">
         <f>G9</f>
-        <v>1.727825E-5</v>
+        <v>6.4793437500000001E-5</v>
       </c>
       <c r="H10" s="31">
         <f>(2*G10)/E10</f>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="J10" s="31">
         <f>(2*G10*K10)/(L10*H10*H10)</f>
-        <v>3.4556499999999993E-5</v>
+        <v>3.2396718749999994E-5</v>
       </c>
       <c r="K10" s="31">
         <v>9.9999999999999995E-7</v>
@@ -2220,15 +2371,15 @@
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G11" s="31">
         <f>S2-G2-G9-G7</f>
-        <v>2.3334350000000004E-4</v>
+        <v>5.9164305555555607E-5</v>
       </c>
       <c r="H11" s="31">
         <f>T2-I2-A2</f>
-        <v>1.3</v>
+        <v>1.25</v>
       </c>
       <c r="J11" s="31">
         <f>(2*G11*K11)/(L11*H11*H11)</f>
-        <v>1.1045846153846153E-5</v>
+        <v>3.0292124444444471E-6</v>
       </c>
       <c r="K11" s="31">
         <v>9.9999999999999995E-7</v>
@@ -2243,22 +2394,22 @@
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E12" s="31">
         <f>F12*G12</f>
-        <v>2.3334350000000005E-3</v>
+        <v>2.9582152777777801E-4</v>
       </c>
       <c r="F12">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G12" s="31">
         <f>G11</f>
-        <v>2.3334350000000004E-4</v>
+        <v>5.9164305555555607E-5</v>
       </c>
       <c r="H12" s="31">
         <f>(2*G12)/E12</f>
-        <v>0.19999999999999998</v>
+        <v>0.4</v>
       </c>
       <c r="J12" s="31">
         <f>(2*G12*K12)/(L12*H12*H12)</f>
-        <v>2.3334350000000009E-4</v>
+        <v>1.47910763888889E-5</v>
       </c>
       <c r="K12" s="31">
         <v>9.9999999999999995E-7</v>
@@ -2281,11 +2432,11 @@
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="31">
         <f>2.5-A2 - H7</f>
-        <v>0.60859782952591313</v>
+        <v>-2.6380072349136228</v>
       </c>
       <c r="B20" s="31">
         <f>-2.5+H6+A2</f>
-        <v>-1.1686577118899821</v>
+        <v>-1.0705310656078924</v>
       </c>
     </row>
   </sheetData>
@@ -2347,4 +2498,706 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="31">
+        <v>2E-3</v>
+      </c>
+      <c r="B2">
+        <v>2.5</v>
+      </c>
+      <c r="C2">
+        <v>-2.5</v>
+      </c>
+      <c r="D2" s="31">
+        <f>((B2*B2)/(A5+B5))-((C2*C2)/(C5+D5))</f>
+        <v>2.1245916700694161E-4</v>
+      </c>
+      <c r="E2" s="31">
+        <f>A2-D2</f>
+        <v>1.7875408329930584E-3</v>
+      </c>
+      <c r="F2" s="31">
+        <f>E2/5</f>
+        <v>3.5750816659861168E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" t="s">
+        <v>125</v>
+      </c>
+      <c r="N4" t="s">
+        <v>126</v>
+      </c>
+      <c r="O4" t="s">
+        <v>127</v>
+      </c>
+      <c r="P4" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>129</v>
+      </c>
+      <c r="R4" t="s">
+        <v>130</v>
+      </c>
+      <c r="S4" t="s">
+        <v>131</v>
+      </c>
+      <c r="T4" t="s">
+        <v>132</v>
+      </c>
+      <c r="U4" t="s">
+        <v>133</v>
+      </c>
+      <c r="V4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="31">
+        <v>9400</v>
+      </c>
+      <c r="B5" s="31">
+        <v>15400</v>
+      </c>
+      <c r="C5" s="31">
+        <v>90000</v>
+      </c>
+      <c r="D5" s="31">
+        <v>68000</v>
+      </c>
+      <c r="F5" s="37">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="G5" s="37">
+        <f>F5/F13</f>
+        <v>0.54462934947049924</v>
+      </c>
+      <c r="L5" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="M5" s="37">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="N5" s="37">
+        <v>0.53669999999999995</v>
+      </c>
+      <c r="O5" s="37">
+        <v>-0.89419999999999999</v>
+      </c>
+      <c r="P5" s="37">
+        <v>-0.78859999999999997</v>
+      </c>
+      <c r="Q5" s="37">
+        <v>-0.73229999999999995</v>
+      </c>
+      <c r="R5" s="37">
+        <v>0.89670000000000005</v>
+      </c>
+      <c r="S5" s="37">
+        <v>0.74439999999999995</v>
+      </c>
+      <c r="T5" s="37">
+        <v>-0.93610000000000004</v>
+      </c>
+      <c r="U5" s="37">
+        <v>0.89670000000000005</v>
+      </c>
+      <c r="V5" s="37">
+        <v>0.14399999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F6" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="G6" s="36"/>
+      <c r="L6" t="s">
+        <v>147</v>
+      </c>
+      <c r="M6" s="31">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="N6" s="31">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="O6" s="41">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="P6" s="31">
+        <v>0.4</v>
+      </c>
+      <c r="Q6" s="31">
+        <v>0.4</v>
+      </c>
+      <c r="R6" s="31">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="S6" s="31">
+        <v>0.4</v>
+      </c>
+      <c r="T6" s="40">
+        <v>1.25</v>
+      </c>
+      <c r="U6" s="31">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="V6" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F7" s="37">
+        <v>6.7999999999999999E-5</v>
+      </c>
+      <c r="G7" s="37">
+        <f>F7/F13</f>
+        <v>0.20574886535552192</v>
+      </c>
+      <c r="L7" t="s">
+        <v>148</v>
+      </c>
+      <c r="M7" s="31">
+        <f>(ABS(M6)-ABS(M5))/ABS(M5)</f>
+        <v>3.6830357142857172E-2</v>
+      </c>
+      <c r="N7" s="31">
+        <f>(ABS(N6)-ABS(N5))/ABS(N5)</f>
+        <v>0.24277995155580417</v>
+      </c>
+      <c r="O7" s="31">
+        <f>(ABS(O6)-ABS(O5))/ABS(O5)</f>
+        <v>4.1889957503914106</v>
+      </c>
+      <c r="P7" s="31">
+        <f>(ABS(P6)-ABS(P5))/ABS(P5)</f>
+        <v>-0.49277200101445595</v>
+      </c>
+      <c r="Q7" s="31">
+        <f>(ABS(Q6)-ABS(Q5))/ABS(Q5)</f>
+        <v>-0.45377577495561922</v>
+      </c>
+      <c r="R7" s="31">
+        <f>(ABS(R6)-ABS(R5))/ABS(R5)</f>
+        <v>3.6020965763354514E-2</v>
+      </c>
+      <c r="S7" s="31">
+        <f>(ABS(S6)-ABS(S5))/ABS(S5)</f>
+        <v>-0.46265448683503485</v>
+      </c>
+      <c r="T7" s="31">
+        <f>(ABS(T6)-ABS(T5))/ABS(T5)</f>
+        <v>0.33532742228394397</v>
+      </c>
+      <c r="U7" s="31">
+        <f>(ABS(U6)-ABS(U5))/ABS(U5)</f>
+        <v>3.6020965763354514E-2</v>
+      </c>
+      <c r="V7" s="31">
+        <f>(ABS(V6)-ABS(V5))/ABS(V5)</f>
+        <v>0.73611111111111127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F8" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" s="36"/>
+      <c r="L8" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="M8" s="37">
+        <v>4.0299999999999998E-4</v>
+      </c>
+      <c r="N8" s="37">
+        <v>6.7299999999999999E-4</v>
+      </c>
+      <c r="O8" s="37">
+        <v>2.7300000000000002E-4</v>
+      </c>
+      <c r="P8" s="37">
+        <v>1.73E-4</v>
+      </c>
+      <c r="Q8" s="37">
+        <v>1.8599999999999999E-4</v>
+      </c>
+      <c r="R8" s="37">
+        <v>1.4200000000000001E-4</v>
+      </c>
+      <c r="S8" s="37">
+        <v>1E-4</v>
+      </c>
+      <c r="T8" s="37">
+        <v>8.0000000000000007E-5</v>
+      </c>
+      <c r="U8" s="37">
+        <v>1E-4</v>
+      </c>
+      <c r="V8" s="37">
+        <v>5.4500000000000002E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F9" s="37">
+        <v>3.7499999999999997E-5</v>
+      </c>
+      <c r="G9" s="37">
+        <f>F9/F13</f>
+        <v>0.11346444780635399</v>
+      </c>
+      <c r="L9" t="s">
+        <v>149</v>
+      </c>
+      <c r="N9" s="31">
+        <v>4.0299999999999998E-4</v>
+      </c>
+      <c r="P9" s="31">
+        <v>3.2400000000000001E-4</v>
+      </c>
+      <c r="Q9" s="31">
+        <v>3.2400000000000001E-4</v>
+      </c>
+      <c r="S9" s="31">
+        <v>2.9599999999999998E-4</v>
+      </c>
+      <c r="V9" s="31">
+        <v>1.73E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F10" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="36"/>
+      <c r="L10" t="s">
+        <v>148</v>
+      </c>
+      <c r="N10" s="31">
+        <f>(ABS(N9)-ABS(N8))/ABS(N8)</f>
+        <v>-0.40118870728083211</v>
+      </c>
+      <c r="P10" s="31">
+        <f>(ABS(P9)-ABS(P8))/ABS(P8)</f>
+        <v>0.8728323699421966</v>
+      </c>
+      <c r="Q10" s="31">
+        <f>(ABS(Q9)-ABS(Q8))/ABS(Q8)</f>
+        <v>0.74193548387096786</v>
+      </c>
+      <c r="S10" s="38">
+        <f>(ABS(S9)-ABS(S8))/ABS(S8)</f>
+        <v>1.9599999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F11" s="37">
+        <v>4.5000000000000003E-5</v>
+      </c>
+      <c r="G11" s="37">
+        <f>F11/F13</f>
+        <v>0.13615733736762481</v>
+      </c>
+      <c r="L11" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="M11" s="37">
+        <v>1.7E-5</v>
+      </c>
+      <c r="N11" s="37">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="O11" s="37">
+        <v>2.3E-5</v>
+      </c>
+      <c r="P11" s="37">
+        <v>7.9999999999999996E-6</v>
+      </c>
+      <c r="Q11" s="37">
+        <v>7.9999999999999996E-6</v>
+      </c>
+      <c r="R11" s="37">
+        <v>6.0000000000000002E-6</v>
+      </c>
+      <c r="S11" s="37">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="T11" s="37">
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="U11" s="37">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="V11" s="37">
+        <v>6.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F12" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="G12" s="36"/>
+      <c r="L12" t="s">
+        <v>153</v>
+      </c>
+      <c r="M12" s="31">
+        <v>1.8700000000000001E-5</v>
+      </c>
+      <c r="N12" s="31">
+        <v>1.2099999999999999E-5</v>
+      </c>
+      <c r="O12" s="39">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="P12" s="31">
+        <v>3.2399999999999999E-6</v>
+      </c>
+      <c r="Q12" s="31">
+        <v>3.2399999999999999E-6</v>
+      </c>
+      <c r="R12" s="31">
+        <v>6.0000000000000002E-6</v>
+      </c>
+      <c r="S12" s="38">
+        <v>1.4800000000000001E-5</v>
+      </c>
+      <c r="T12" s="31">
+        <v>3.0299999999999998E-6</v>
+      </c>
+      <c r="U12" s="31">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="V12" s="31">
+        <v>1.38E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F13" s="37">
+        <f>F5+F7+F9+F11</f>
+        <v>3.3050000000000001E-4</v>
+      </c>
+      <c r="G13" s="36"/>
+      <c r="L13" s="36" t="s">
+        <v>154</v>
+      </c>
+      <c r="M13" s="37">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="N13" s="37">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="O13" s="37">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="P13" s="37">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="Q13" s="37">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="R13" s="37">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="S13" s="37">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="T13" s="37">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="U13" s="37">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="V13" s="37">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>155</v>
+      </c>
+      <c r="M14" s="31">
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="N14" s="31">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="O14" s="31">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="P14" s="31">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="Q14" s="31">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="R14" s="31">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="S14" s="31">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="T14" s="31">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="U14" s="31">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="V14" s="31">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F16" t="s">
+        <v>136</v>
+      </c>
+      <c r="G16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H16" t="s">
+        <v>138</v>
+      </c>
+      <c r="I16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="E17" s="37">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="F17" s="37">
+        <v>6.7999999999999999E-5</v>
+      </c>
+      <c r="G17" s="37">
+        <v>3.7499999999999997E-5</v>
+      </c>
+      <c r="H17" s="37">
+        <v>4.5000000000000003E-5</v>
+      </c>
+      <c r="I17" s="37">
+        <f>E17+F17+G17+H17</f>
+        <v>3.3050000000000001E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="E18" s="37">
+        <f>E17/I17</f>
+        <v>0.54462934947049924</v>
+      </c>
+      <c r="F18" s="37">
+        <f>F17/I17</f>
+        <v>0.20574886535552192</v>
+      </c>
+      <c r="G18" s="37">
+        <f>G17/I17</f>
+        <v>0.11346444780635399</v>
+      </c>
+      <c r="H18" s="37">
+        <f>H17/I17</f>
+        <v>0.13615733736762481</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>139</v>
+      </c>
+      <c r="E19">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F19">
+        <v>0.2</v>
+      </c>
+      <c r="G19">
+        <v>0.1</v>
+      </c>
+      <c r="H19">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>151</v>
+      </c>
+      <c r="E20" s="31">
+        <f>F2*E19</f>
+        <v>1.9662949162923643E-4</v>
+      </c>
+      <c r="F20" s="31">
+        <f>F2*F19</f>
+        <v>7.1501633319722341E-5</v>
+      </c>
+      <c r="G20" s="31">
+        <f>F2*G19</f>
+        <v>3.575081665986117E-5</v>
+      </c>
+      <c r="H20" s="31">
+        <f>F2*H19</f>
+        <v>5.3626224989791749E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" s="31">
+        <v>1.34E-4</v>
+      </c>
+      <c r="F21" s="31">
+        <v>6.4800000000000003E-5</v>
+      </c>
+      <c r="G21" s="38">
+        <v>5.9200000000000002E-5</v>
+      </c>
+      <c r="H21" s="31">
+        <v>2.16E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>148</v>
+      </c>
+      <c r="E22" s="31">
+        <f>(E21-E17)/E17</f>
+        <v>-0.25555555555555559</v>
+      </c>
+      <c r="F22" s="31">
+        <f t="shared" ref="F22:H22" si="0">(F21-F17)/F17</f>
+        <v>-4.7058823529411715E-2</v>
+      </c>
+      <c r="G22" s="31">
+        <f t="shared" si="0"/>
+        <v>0.57866666666666688</v>
+      </c>
+      <c r="H22" s="31">
+        <f t="shared" si="0"/>
+        <v>-0.52</v>
+      </c>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="E23" s="36">
+        <v>74.941400000000002</v>
+      </c>
+      <c r="F23" s="36">
+        <v>90.259900000000002</v>
+      </c>
+      <c r="G23" s="37">
+        <v>91.618600000000001</v>
+      </c>
+      <c r="H23" s="36">
+        <v>89.548100000000005</v>
+      </c>
+      <c r="I23" s="31">
+        <f>E23*F23*G23*H23</f>
+        <v>55495360.476850562</v>
+      </c>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D24" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="E24">
+        <f>POWER(10,E23/20)</f>
+        <v>5585.6021675172306</v>
+      </c>
+      <c r="F24">
+        <f>POWER(10,F23/20)</f>
+        <v>32583.29496899508</v>
+      </c>
+      <c r="G24">
+        <f>POWER(10,G23/20)</f>
+        <v>38100.440778951204</v>
+      </c>
+      <c r="H24">
+        <f>POWER(10,H23/20)</f>
+        <v>30019.606833923423</v>
+      </c>
+    </row>
+    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D25" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="E25" s="37">
+        <v>200546600</v>
+      </c>
+      <c r="F25" s="37">
+        <v>114422200</v>
+      </c>
+      <c r="G25" s="37">
+        <v>104984600</v>
+      </c>
+      <c r="H25" s="37">
+        <v>96613300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
first draft of page 3-6
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="75" windowWidth="19155" windowHeight="7740" activeTab="3"/>
+    <workbookView xWindow="1410" yWindow="75" windowWidth="19155" windowHeight="7740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="164">
   <si>
     <t>node</t>
   </si>
@@ -514,6 +514,30 @@
   </si>
   <si>
     <t>calc L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kn </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp </t>
+  </si>
+  <si>
+    <t>vss</t>
+  </si>
+  <si>
+    <t>Vy</t>
+  </si>
+  <si>
+    <t>Id8</t>
+  </si>
+  <si>
+    <t>Vz</t>
+  </si>
+  <si>
+    <t>Vov8</t>
+  </si>
+  <si>
+    <t>Vov7</t>
   </si>
 </sst>
 </file>
@@ -785,16 +809,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1350,16 +1374,16 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="34"/>
-      <c r="E20" s="32" t="s">
+      <c r="B20" s="39"/>
+      <c r="C20" s="40"/>
+      <c r="E20" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="33"/>
-      <c r="G20" s="34"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="40"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -1433,11 +1457,11 @@
       <c r="C24" s="9"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
@@ -2036,10 +2060,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2437,6 +2461,90 @@
       <c r="B20" s="31">
         <f>-2.5+H6+A2</f>
         <v>-1.0705310656078924</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>161</v>
+      </c>
+      <c r="B22">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>156</v>
+      </c>
+      <c r="B24" s="31">
+        <v>5.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>157</v>
+      </c>
+      <c r="B25" s="31">
+        <v>2.5000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>158</v>
+      </c>
+      <c r="B27" s="31">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>160</v>
+      </c>
+      <c r="B28" s="31">
+        <f>0.5*B25*1*POWER(B29, 2)</f>
+        <v>8.0000000000000013E-6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>162</v>
+      </c>
+      <c r="B29" s="31">
+        <f>B26-B22-B23</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>163</v>
+      </c>
+      <c r="B30" s="31">
+        <f>SQRT(B28*2/B24)</f>
+        <v>0.56568542494923812</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>159</v>
+      </c>
+      <c r="B31" s="31">
+        <f>B30-B27-B23</f>
+        <v>2.5656854249492382</v>
       </c>
     </row>
   </sheetData>
@@ -2504,7 +2612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -2574,10 +2682,10 @@
       <c r="D4" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="32" t="s">
         <v>6</v>
       </c>
       <c r="M4" t="s">
@@ -2624,52 +2732,52 @@
       <c r="D5" s="31">
         <v>68000</v>
       </c>
-      <c r="F5" s="37">
+      <c r="F5" s="33">
         <v>1.8000000000000001E-4</v>
       </c>
-      <c r="G5" s="37">
+      <c r="G5" s="33">
         <f>F5/F13</f>
         <v>0.54462934947049924</v>
       </c>
-      <c r="L5" s="36" t="s">
+      <c r="L5" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="M5" s="37">
+      <c r="M5" s="33">
         <v>0.89600000000000002</v>
       </c>
-      <c r="N5" s="37">
+      <c r="N5" s="33">
         <v>0.53669999999999995</v>
       </c>
-      <c r="O5" s="37">
+      <c r="O5" s="33">
         <v>-0.89419999999999999</v>
       </c>
-      <c r="P5" s="37">
+      <c r="P5" s="33">
         <v>-0.78859999999999997</v>
       </c>
-      <c r="Q5" s="37">
+      <c r="Q5" s="33">
         <v>-0.73229999999999995</v>
       </c>
-      <c r="R5" s="37">
+      <c r="R5" s="33">
         <v>0.89670000000000005</v>
       </c>
-      <c r="S5" s="37">
+      <c r="S5" s="33">
         <v>0.74439999999999995</v>
       </c>
-      <c r="T5" s="37">
+      <c r="T5" s="33">
         <v>-0.93610000000000004</v>
       </c>
-      <c r="U5" s="37">
+      <c r="U5" s="33">
         <v>0.89670000000000005</v>
       </c>
-      <c r="V5" s="37">
+      <c r="V5" s="33">
         <v>0.14399999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="G6" s="36"/>
+      <c r="G6" s="32"/>
       <c r="L6" t="s">
         <v>147</v>
       </c>
@@ -2679,7 +2787,7 @@
       <c r="N6" s="31">
         <v>0.66700000000000004</v>
       </c>
-      <c r="O6" s="41">
+      <c r="O6" s="37">
         <v>4.6399999999999997</v>
       </c>
       <c r="P6" s="31">
@@ -2694,7 +2802,7 @@
       <c r="S6" s="31">
         <v>0.4</v>
       </c>
-      <c r="T6" s="40">
+      <c r="T6" s="36">
         <v>1.25</v>
       </c>
       <c r="U6" s="31">
@@ -2705,10 +2813,10 @@
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F7" s="37">
+      <c r="F7" s="33">
         <v>6.7999999999999999E-5</v>
       </c>
-      <c r="G7" s="37">
+      <c r="G7" s="33">
         <f>F7/F13</f>
         <v>0.20574886535552192</v>
       </c>
@@ -2716,90 +2824,90 @@
         <v>148</v>
       </c>
       <c r="M7" s="31">
-        <f>(ABS(M6)-ABS(M5))/ABS(M5)</f>
+        <f t="shared" ref="M7:V7" si="0">(ABS(M6)-ABS(M5))/ABS(M5)</f>
         <v>3.6830357142857172E-2</v>
       </c>
       <c r="N7" s="31">
-        <f>(ABS(N6)-ABS(N5))/ABS(N5)</f>
+        <f t="shared" si="0"/>
         <v>0.24277995155580417</v>
       </c>
       <c r="O7" s="31">
-        <f>(ABS(O6)-ABS(O5))/ABS(O5)</f>
+        <f t="shared" si="0"/>
         <v>4.1889957503914106</v>
       </c>
       <c r="P7" s="31">
-        <f>(ABS(P6)-ABS(P5))/ABS(P5)</f>
+        <f t="shared" si="0"/>
         <v>-0.49277200101445595</v>
       </c>
       <c r="Q7" s="31">
-        <f>(ABS(Q6)-ABS(Q5))/ABS(Q5)</f>
+        <f t="shared" si="0"/>
         <v>-0.45377577495561922</v>
       </c>
       <c r="R7" s="31">
-        <f>(ABS(R6)-ABS(R5))/ABS(R5)</f>
+        <f t="shared" si="0"/>
         <v>3.6020965763354514E-2</v>
       </c>
       <c r="S7" s="31">
-        <f>(ABS(S6)-ABS(S5))/ABS(S5)</f>
+        <f t="shared" si="0"/>
         <v>-0.46265448683503485</v>
       </c>
       <c r="T7" s="31">
-        <f>(ABS(T6)-ABS(T5))/ABS(T5)</f>
+        <f t="shared" si="0"/>
         <v>0.33532742228394397</v>
       </c>
       <c r="U7" s="31">
-        <f>(ABS(U6)-ABS(U5))/ABS(U5)</f>
+        <f t="shared" si="0"/>
         <v>3.6020965763354514E-2</v>
       </c>
       <c r="V7" s="31">
-        <f>(ABS(V6)-ABS(V5))/ABS(V5)</f>
+        <f t="shared" si="0"/>
         <v>0.73611111111111127</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="G8" s="36"/>
-      <c r="L8" s="36" t="s">
+      <c r="G8" s="32"/>
+      <c r="L8" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="M8" s="37">
+      <c r="M8" s="33">
         <v>4.0299999999999998E-4</v>
       </c>
-      <c r="N8" s="37">
+      <c r="N8" s="33">
         <v>6.7299999999999999E-4</v>
       </c>
-      <c r="O8" s="37">
+      <c r="O8" s="33">
         <v>2.7300000000000002E-4</v>
       </c>
-      <c r="P8" s="37">
+      <c r="P8" s="33">
         <v>1.73E-4</v>
       </c>
-      <c r="Q8" s="37">
+      <c r="Q8" s="33">
         <v>1.8599999999999999E-4</v>
       </c>
-      <c r="R8" s="37">
+      <c r="R8" s="33">
         <v>1.4200000000000001E-4</v>
       </c>
-      <c r="S8" s="37">
+      <c r="S8" s="33">
         <v>1E-4</v>
       </c>
-      <c r="T8" s="37">
+      <c r="T8" s="33">
         <v>8.0000000000000007E-5</v>
       </c>
-      <c r="U8" s="37">
+      <c r="U8" s="33">
         <v>1E-4</v>
       </c>
-      <c r="V8" s="37">
+      <c r="V8" s="33">
         <v>5.4500000000000002E-4</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F9" s="37">
+      <c r="F9" s="33">
         <v>3.7499999999999997E-5</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9" s="33">
         <f>F9/F13</f>
         <v>0.11346444780635399</v>
       </c>
@@ -2823,10 +2931,10 @@
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F10" s="36" t="s">
+      <c r="F10" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="G10" s="36"/>
+      <c r="G10" s="32"/>
       <c r="L10" t="s">
         <v>148</v>
       </c>
@@ -2842,58 +2950,58 @@
         <f>(ABS(Q9)-ABS(Q8))/ABS(Q8)</f>
         <v>0.74193548387096786</v>
       </c>
-      <c r="S10" s="38">
+      <c r="S10" s="34">
         <f>(ABS(S9)-ABS(S8))/ABS(S8)</f>
         <v>1.9599999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F11" s="37">
+      <c r="F11" s="33">
         <v>4.5000000000000003E-5</v>
       </c>
-      <c r="G11" s="37">
+      <c r="G11" s="33">
         <f>F11/F13</f>
         <v>0.13615733736762481</v>
       </c>
-      <c r="L11" s="36" t="s">
+      <c r="L11" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="M11" s="37">
+      <c r="M11" s="33">
         <v>1.7E-5</v>
       </c>
-      <c r="N11" s="37">
+      <c r="N11" s="33">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="O11" s="37">
+      <c r="O11" s="33">
         <v>2.3E-5</v>
       </c>
-      <c r="P11" s="37">
+      <c r="P11" s="33">
         <v>7.9999999999999996E-6</v>
       </c>
-      <c r="Q11" s="37">
+      <c r="Q11" s="33">
         <v>7.9999999999999996E-6</v>
       </c>
-      <c r="R11" s="37">
+      <c r="R11" s="33">
         <v>6.0000000000000002E-6</v>
       </c>
-      <c r="S11" s="37">
+      <c r="S11" s="33">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="T11" s="37">
+      <c r="T11" s="33">
         <v>3.0000000000000001E-6</v>
       </c>
-      <c r="U11" s="37">
+      <c r="U11" s="33">
         <v>3.9999999999999998E-6</v>
       </c>
-      <c r="V11" s="37">
+      <c r="V11" s="33">
         <v>6.0000000000000002E-5</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F12" s="36" t="s">
+      <c r="F12" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="G12" s="36"/>
+      <c r="G12" s="32"/>
       <c r="L12" t="s">
         <v>153</v>
       </c>
@@ -2903,7 +3011,7 @@
       <c r="N12" s="31">
         <v>1.2099999999999999E-5</v>
       </c>
-      <c r="O12" s="39">
+      <c r="O12" s="35">
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="P12" s="31">
@@ -2915,7 +3023,7 @@
       <c r="R12" s="31">
         <v>6.0000000000000002E-6</v>
       </c>
-      <c r="S12" s="38">
+      <c r="S12" s="34">
         <v>1.4800000000000001E-5</v>
       </c>
       <c r="T12" s="31">
@@ -2929,42 +3037,42 @@
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F13" s="37">
+      <c r="F13" s="33">
         <f>F5+F7+F9+F11</f>
         <v>3.3050000000000001E-4</v>
       </c>
-      <c r="G13" s="36"/>
-      <c r="L13" s="36" t="s">
+      <c r="G13" s="32"/>
+      <c r="L13" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="M13" s="37">
+      <c r="M13" s="33">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="N13" s="37">
+      <c r="N13" s="33">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="O13" s="37">
+      <c r="O13" s="33">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="P13" s="37">
+      <c r="P13" s="33">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="Q13" s="37">
+      <c r="Q13" s="33">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="R13" s="37">
+      <c r="R13" s="33">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="S13" s="37">
+      <c r="S13" s="33">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="T13" s="37">
+      <c r="T13" s="33">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="U13" s="37">
+      <c r="U13" s="33">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="V13" s="37">
+      <c r="V13" s="33">
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
@@ -3021,43 +3129,43 @@
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="E17" s="37">
+      <c r="E17" s="33">
         <v>1.8000000000000001E-4</v>
       </c>
-      <c r="F17" s="37">
+      <c r="F17" s="33">
         <v>6.7999999999999999E-5</v>
       </c>
-      <c r="G17" s="37">
+      <c r="G17" s="33">
         <v>3.7499999999999997E-5</v>
       </c>
-      <c r="H17" s="37">
+      <c r="H17" s="33">
         <v>4.5000000000000003E-5</v>
       </c>
-      <c r="I17" s="37">
+      <c r="I17" s="33">
         <f>E17+F17+G17+H17</f>
         <v>3.3050000000000001E-4</v>
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D18" s="36" t="s">
+      <c r="D18" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="E18" s="37">
+      <c r="E18" s="33">
         <f>E17/I17</f>
         <v>0.54462934947049924</v>
       </c>
-      <c r="F18" s="37">
+      <c r="F18" s="33">
         <f>F17/I17</f>
         <v>0.20574886535552192</v>
       </c>
-      <c r="G18" s="37">
+      <c r="G18" s="33">
         <f>G17/I17</f>
         <v>0.11346444780635399</v>
       </c>
-      <c r="H18" s="37">
+      <c r="H18" s="33">
         <f>H17/I17</f>
         <v>0.13615733736762481</v>
       </c>
@@ -3110,7 +3218,7 @@
       <c r="F21" s="31">
         <v>6.4800000000000003E-5</v>
       </c>
-      <c r="G21" s="38">
+      <c r="G21" s="34">
         <v>5.9200000000000002E-5</v>
       </c>
       <c r="H21" s="31">
@@ -3126,32 +3234,32 @@
         <v>-0.25555555555555559</v>
       </c>
       <c r="F22" s="31">
-        <f t="shared" ref="F22:H22" si="0">(F21-F17)/F17</f>
+        <f t="shared" ref="F22:H22" si="1">(F21-F17)/F17</f>
         <v>-4.7058823529411715E-2</v>
       </c>
       <c r="G22" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.57866666666666688</v>
       </c>
       <c r="H22" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.52</v>
       </c>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D23" s="36" t="s">
+      <c r="D23" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="E23" s="36">
+      <c r="E23" s="32">
         <v>74.941400000000002</v>
       </c>
-      <c r="F23" s="36">
+      <c r="F23" s="32">
         <v>90.259900000000002</v>
       </c>
-      <c r="G23" s="37">
+      <c r="G23" s="33">
         <v>91.618600000000001</v>
       </c>
-      <c r="H23" s="36">
+      <c r="H23" s="32">
         <v>89.548100000000005</v>
       </c>
       <c r="I23" s="31">
@@ -3160,7 +3268,7 @@
       </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D24" s="36" t="s">
+      <c r="D24" s="32" t="s">
         <v>145</v>
       </c>
       <c r="E24">
@@ -3181,19 +3289,19 @@
       </c>
     </row>
     <row r="25" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D25" s="36" t="s">
+      <c r="D25" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="E25" s="37">
+      <c r="E25" s="33">
         <v>200546600</v>
       </c>
-      <c r="F25" s="37">
+      <c r="F25" s="33">
         <v>114422200</v>
       </c>
-      <c r="G25" s="37">
+      <c r="G25" s="33">
         <v>104984600</v>
       </c>
-      <c r="H25" s="37">
+      <c r="H25" s="33">
         <v>96613300</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made lots of changes to design doc and squeezed it into the pages that they want
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruggler\Desktop\project214\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="75" windowWidth="19155" windowHeight="7740" activeTab="3"/>
+    <workbookView xWindow="3270" yWindow="75" windowWidth="19155" windowHeight="7740" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -450,9 +455,6 @@
     <t>M9</t>
   </si>
   <si>
-    <t>spice Vov</t>
-  </si>
-  <si>
     <t>stack1</t>
   </si>
   <si>
@@ -486,34 +488,13 @@
     <t>spice gain in ohms</t>
   </si>
   <si>
-    <t>spice gm</t>
-  </si>
-  <si>
-    <t>calc Vov</t>
-  </si>
-  <si>
     <t>% error</t>
   </si>
   <si>
-    <t>calc gm</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ids </t>
   </si>
   <si>
     <t>Ids allocated</t>
-  </si>
-  <si>
-    <t>spice W</t>
-  </si>
-  <si>
-    <t>calc W</t>
-  </si>
-  <si>
-    <t>spice L</t>
-  </si>
-  <si>
-    <t>calc L</t>
   </si>
   <si>
     <t xml:space="preserve">kn </t>
@@ -569,12 +550,39 @@
   <si>
     <t>total power
  dissipated</t>
+  </si>
+  <si>
+    <t>SPICE Id (uA)</t>
+  </si>
+  <si>
+    <t>Computed Id (uA)</t>
+  </si>
+  <si>
+    <t>Final W (um)</t>
+  </si>
+  <si>
+    <t>Computed W (um)</t>
+  </si>
+  <si>
+    <t>Final L (um)</t>
+  </si>
+  <si>
+    <t>Computed L (um)</t>
+  </si>
+  <si>
+    <t>SPICE Vov (V)</t>
+  </si>
+  <si>
+    <t>Computed Vov (V)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -605,7 +613,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -618,14 +626,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -791,11 +793,215 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -843,12 +1049,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -858,6 +1059,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -961,7 +1184,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -996,7 +1219,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1413,16 +1636,16 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="39"/>
-      <c r="E20" s="37" t="s">
+      <c r="B20" s="40"/>
+      <c r="C20" s="41"/>
+      <c r="E20" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="38"/>
-      <c r="G20" s="39"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="41"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -1496,11 +1719,11 @@
       <c r="C24" s="9"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="40" t="s">
+      <c r="A26" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="40"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
@@ -2102,7 +2325,7 @@
   <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2504,7 +2727,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B22">
         <v>1.2</v>
@@ -2520,7 +2743,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B24" s="31">
         <v>5.0000000000000002E-5</v>
@@ -2528,7 +2751,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B25" s="31">
         <v>2.5000000000000001E-5</v>
@@ -2544,7 +2767,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B27" s="31">
         <v>-2.5</v>
@@ -2552,7 +2775,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B28" s="31">
         <f>0.5*B25*1*POWER(B29, 2)</f>
@@ -2561,7 +2784,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B29" s="31">
         <f>B26-B22-B23</f>
@@ -2570,7 +2793,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B30" s="31">
         <f>SQRT(B28*2/B24)</f>
@@ -2579,11 +2802,11 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B31" s="31">
-        <f>B30-B27-B23</f>
-        <v>2.5656854249492382</v>
+        <f>(B30+B27-B23)/SQRT(2)</f>
+        <v>-1.7213203435596423</v>
       </c>
     </row>
   </sheetData>
@@ -2651,8 +2874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Y18" sqref="Y18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2666,6 +2889,8 @@
     <col min="7" max="7" width="9.28515625" customWidth="1"/>
     <col min="8" max="9" width="9.5703125" customWidth="1"/>
     <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" customWidth="1"/>
+    <col min="13" max="22" width="7.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -2711,7 +2936,8 @@
         <v>3.416853817884851E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -2730,34 +2956,35 @@
       <c r="G4" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="M4" t="s">
+      <c r="L4" s="43"/>
+      <c r="M4" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="44" t="s">
         <v>127</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S4" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T4" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="U4" t="s">
+      <c r="U4" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="V4" t="s">
+      <c r="V4" s="45" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2781,37 +3008,37 @@
         <f>F5/F13</f>
         <v>0.54462934947049924</v>
       </c>
-      <c r="L5" s="32" t="s">
-        <v>134</v>
-      </c>
-      <c r="M5" s="33">
+      <c r="L5" s="46" t="s">
+        <v>172</v>
+      </c>
+      <c r="M5" s="51">
         <v>0.89600000000000002</v>
       </c>
-      <c r="N5" s="33">
+      <c r="N5" s="51">
         <v>0.53669999999999995</v>
       </c>
-      <c r="O5" s="33">
-        <v>-0.89419999999999999</v>
-      </c>
-      <c r="P5" s="33">
-        <v>-0.78859999999999997</v>
-      </c>
-      <c r="Q5" s="33">
-        <v>-0.73229999999999995</v>
-      </c>
-      <c r="R5" s="33">
+      <c r="O5" s="51">
+        <v>0.89419999999999999</v>
+      </c>
+      <c r="P5" s="51">
+        <v>0.78859999999999997</v>
+      </c>
+      <c r="Q5" s="51">
+        <v>0.73229999999999995</v>
+      </c>
+      <c r="R5" s="51">
         <v>0.89670000000000005</v>
       </c>
-      <c r="S5" s="33">
+      <c r="S5" s="51">
         <v>0.74439999999999995</v>
       </c>
-      <c r="T5" s="33">
-        <v>-0.93610000000000004</v>
-      </c>
-      <c r="U5" s="33">
+      <c r="T5" s="51">
+        <v>0.93610000000000004</v>
+      </c>
+      <c r="U5" s="51">
         <v>0.89670000000000005</v>
       </c>
-      <c r="V5" s="33">
+      <c r="V5" s="52">
         <v>0.14399999999999999</v>
       </c>
     </row>
@@ -2820,41 +3047,41 @@
         <v>121</v>
       </c>
       <c r="G6" s="32"/>
-      <c r="L6" t="s">
-        <v>147</v>
-      </c>
-      <c r="M6" s="31">
+      <c r="L6" s="47" t="s">
+        <v>173</v>
+      </c>
+      <c r="M6" s="53">
         <v>0.92900000000000005</v>
       </c>
-      <c r="N6" s="31">
+      <c r="N6" s="53">
         <v>0.66700000000000004</v>
       </c>
-      <c r="O6" s="36">
+      <c r="O6" s="53">
         <v>4.6399999999999997</v>
       </c>
-      <c r="P6" s="31">
+      <c r="P6" s="53">
         <v>0.4</v>
       </c>
-      <c r="Q6" s="31">
+      <c r="Q6" s="53">
         <v>0.4</v>
       </c>
-      <c r="R6" s="31">
+      <c r="R6" s="53">
         <v>0.92900000000000005</v>
       </c>
-      <c r="S6" s="31">
+      <c r="S6" s="53">
         <v>0.4</v>
       </c>
-      <c r="T6" s="35">
+      <c r="T6" s="53">
         <v>1.25</v>
       </c>
-      <c r="U6" s="31">
+      <c r="U6" s="53">
         <v>0.92900000000000005</v>
       </c>
-      <c r="V6" s="31">
+      <c r="V6" s="54">
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F7" s="33">
         <v>6.7999999999999999E-5</v>
       </c>
@@ -2862,46 +3089,46 @@
         <f>F7/F13</f>
         <v>0.20574886535552192</v>
       </c>
-      <c r="L7" t="s">
-        <v>148</v>
-      </c>
-      <c r="M7" s="31">
-        <f t="shared" ref="M7:V7" si="0">(ABS(M6)-ABS(M5))/ABS(M5)</f>
+      <c r="L7" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="M7" s="50">
+        <f>(ABS(M6-M5))/ABS(M5)</f>
         <v>3.6830357142857172E-2</v>
       </c>
-      <c r="N7" s="31">
-        <f t="shared" si="0"/>
+      <c r="N7" s="50">
+        <f t="shared" ref="N7:V7" si="0">(ABS(N6-N5))/ABS(N5)</f>
         <v>0.24277995155580417</v>
       </c>
-      <c r="O7" s="31">
+      <c r="O7" s="50">
         <f t="shared" si="0"/>
         <v>4.1889957503914106</v>
       </c>
-      <c r="P7" s="31">
+      <c r="P7" s="50">
         <f t="shared" si="0"/>
-        <v>-0.49277200101445595</v>
-      </c>
-      <c r="Q7" s="31">
+        <v>0.49277200101445595</v>
+      </c>
+      <c r="Q7" s="50">
         <f t="shared" si="0"/>
-        <v>-0.45377577495561922</v>
-      </c>
-      <c r="R7" s="31">
+        <v>0.45377577495561922</v>
+      </c>
+      <c r="R7" s="50">
         <f t="shared" si="0"/>
         <v>3.6020965763354514E-2</v>
       </c>
-      <c r="S7" s="31">
+      <c r="S7" s="50">
         <f t="shared" si="0"/>
-        <v>-0.46265448683503485</v>
-      </c>
-      <c r="T7" s="31">
+        <v>0.46265448683503485</v>
+      </c>
+      <c r="T7" s="50">
         <f t="shared" si="0"/>
         <v>0.33532742228394397</v>
       </c>
-      <c r="U7" s="31">
+      <c r="U7" s="50">
         <f t="shared" si="0"/>
         <v>3.6020965763354514E-2</v>
       </c>
-      <c r="V7" s="31">
+      <c r="V7" s="50">
         <f t="shared" si="0"/>
         <v>0.73611111111111127</v>
       </c>
@@ -2911,38 +3138,38 @@
         <v>122</v>
       </c>
       <c r="G8" s="32"/>
-      <c r="L8" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="M8" s="33">
-        <v>4.0299999999999998E-4</v>
-      </c>
-      <c r="N8" s="33">
-        <v>6.7299999999999999E-4</v>
-      </c>
-      <c r="O8" s="33">
-        <v>2.7300000000000002E-4</v>
-      </c>
-      <c r="P8" s="33">
-        <v>1.73E-4</v>
-      </c>
-      <c r="Q8" s="33">
-        <v>1.8599999999999999E-4</v>
-      </c>
-      <c r="R8" s="33">
-        <v>1.4200000000000001E-4</v>
-      </c>
-      <c r="S8" s="33">
-        <v>1E-4</v>
-      </c>
-      <c r="T8" s="33">
-        <v>8.0000000000000007E-5</v>
-      </c>
-      <c r="U8" s="33">
-        <v>1E-4</v>
-      </c>
-      <c r="V8" s="33">
-        <v>5.4500000000000002E-4</v>
+      <c r="L8" s="46" t="s">
+        <v>166</v>
+      </c>
+      <c r="M8" s="51">
+        <v>180.8</v>
+      </c>
+      <c r="N8" s="51">
+        <v>180.8</v>
+      </c>
+      <c r="O8" s="51">
+        <v>122.4</v>
+      </c>
+      <c r="P8" s="51">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="Q8" s="51">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="R8" s="51">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="S8" s="51">
+        <v>37.6</v>
+      </c>
+      <c r="T8" s="51">
+        <v>37.6</v>
+      </c>
+      <c r="U8" s="51">
+        <v>45</v>
+      </c>
+      <c r="V8" s="52">
+        <v>39.299999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -2953,48 +3180,97 @@
         <f>F9/F13</f>
         <v>0.11346444780635399</v>
       </c>
-      <c r="L9" t="s">
-        <v>149</v>
-      </c>
-      <c r="N9" s="31">
-        <v>4.0299999999999998E-4</v>
-      </c>
-      <c r="P9" s="31">
-        <v>3.2400000000000001E-4</v>
-      </c>
-      <c r="Q9" s="31">
-        <v>3.2400000000000001E-4</v>
-      </c>
-      <c r="S9" s="31">
-        <v>2.9599999999999998E-4</v>
-      </c>
-      <c r="V9" s="31">
-        <v>1.73E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L9" s="47" t="s">
+        <v>167</v>
+      </c>
+      <c r="M9" s="53">
+        <f>M5^2*0.5*0.00005*M12/M14*1000000</f>
+        <v>125.10549333333333</v>
+      </c>
+      <c r="N9" s="53">
+        <f t="shared" ref="N9:V9" si="1">N5^2*0.5*0.00005*N12/N14*1000000</f>
+        <v>87.134184224999984</v>
+      </c>
+      <c r="O9" s="53">
+        <f>O5^2*0.5*0.000025*O12/O14*1000000</f>
+        <v>19.989841000000002</v>
+      </c>
+      <c r="P9" s="53">
+        <f>P5^2*0.5*0.000025*P12/P14*1000000</f>
+        <v>25.186543379999996</v>
+      </c>
+      <c r="Q9" s="53">
+        <f>Q5^2*0.5*0.000025*Q12/Q14*1000000</f>
+        <v>21.718663244999998</v>
+      </c>
+      <c r="R9" s="53">
+        <f t="shared" si="1"/>
+        <v>60.30531675000001</v>
+      </c>
+      <c r="S9" s="53">
+        <f t="shared" si="1"/>
+        <v>205.02860320000002</v>
+      </c>
+      <c r="T9" s="53">
+        <f>T5^2*0.5*0.000025*T12/T14*1000000</f>
+        <v>33.189226578750002</v>
+      </c>
+      <c r="U9" s="53">
+        <f t="shared" si="1"/>
+        <v>20.101772250000003</v>
+      </c>
+      <c r="V9" s="53">
+        <f t="shared" si="1"/>
+        <v>7.1539200000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F10" s="32" t="s">
         <v>123</v>
       </c>
       <c r="G10" s="32"/>
-      <c r="L10" t="s">
-        <v>148</v>
-      </c>
-      <c r="N10" s="31">
-        <f>(ABS(N9)-ABS(N8))/ABS(N8)</f>
-        <v>-0.40118870728083211</v>
-      </c>
-      <c r="P10" s="31">
-        <f>(ABS(P9)-ABS(P8))/ABS(P8)</f>
-        <v>0.8728323699421966</v>
-      </c>
-      <c r="Q10" s="31">
-        <f>(ABS(Q9)-ABS(Q8))/ABS(Q8)</f>
-        <v>0.74193548387096786</v>
-      </c>
-      <c r="S10" s="34">
-        <f>(ABS(S9)-ABS(S8))/ABS(S8)</f>
-        <v>1.9599999999999997</v>
+      <c r="L10" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="M10" s="50">
+        <f>(ABS(M9-M8))/ABS(M8)</f>
+        <v>0.30804483775811214</v>
+      </c>
+      <c r="N10" s="50">
+        <f>(ABS(N9-N8))/ABS(N8)</f>
+        <v>0.51806314034845147</v>
+      </c>
+      <c r="O10" s="50">
+        <f>(ABS(O9-O8))/ABS(O8)</f>
+        <v>0.83668430555555562</v>
+      </c>
+      <c r="P10" s="50">
+        <f t="shared" ref="P10:V10" si="2">(ABS(P9-P8))/ABS(P8)</f>
+        <v>0.63177568157894748</v>
+      </c>
+      <c r="Q10" s="50">
+        <f t="shared" si="2"/>
+        <v>0.68247568355263155</v>
+      </c>
+      <c r="R10" s="50">
+        <f t="shared" si="2"/>
+        <v>5.919942667706684E-2</v>
+      </c>
+      <c r="S10" s="50">
+        <f t="shared" si="2"/>
+        <v>4.452888382978724</v>
+      </c>
+      <c r="T10" s="50">
+        <f t="shared" si="2"/>
+        <v>0.11730780375664891</v>
+      </c>
+      <c r="U10" s="50">
+        <f t="shared" si="2"/>
+        <v>0.55329394999999992</v>
+      </c>
+      <c r="V10" s="50">
+        <f t="shared" si="2"/>
+        <v>0.81796641221374045</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -3005,77 +3281,77 @@
         <f>F11/F13</f>
         <v>0.13615733736762481</v>
       </c>
-      <c r="L11" s="32" t="s">
-        <v>152</v>
-      </c>
-      <c r="M11" s="33">
-        <v>1.7E-5</v>
-      </c>
-      <c r="N11" s="33">
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="O11" s="33">
-        <v>2.3E-5</v>
-      </c>
-      <c r="P11" s="33">
-        <v>7.9999999999999996E-6</v>
-      </c>
-      <c r="Q11" s="33">
-        <v>7.9999999999999996E-6</v>
-      </c>
-      <c r="R11" s="33">
-        <v>6.0000000000000002E-6</v>
-      </c>
-      <c r="S11" s="33">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="T11" s="33">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="U11" s="33">
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="V11" s="33">
-        <v>6.0000000000000002E-5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L11" s="46" t="s">
+        <v>168</v>
+      </c>
+      <c r="M11" s="55">
+        <v>17</v>
+      </c>
+      <c r="N11" s="55">
+        <v>20</v>
+      </c>
+      <c r="O11" s="55">
+        <v>23</v>
+      </c>
+      <c r="P11" s="55">
+        <v>8</v>
+      </c>
+      <c r="Q11" s="55">
+        <v>8</v>
+      </c>
+      <c r="R11" s="55">
+        <v>6</v>
+      </c>
+      <c r="S11" s="55">
+        <v>2</v>
+      </c>
+      <c r="T11" s="55">
+        <v>3</v>
+      </c>
+      <c r="U11" s="55">
+        <v>4</v>
+      </c>
+      <c r="V11" s="56">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F12" s="32" t="s">
         <v>124</v>
       </c>
       <c r="G12" s="32"/>
-      <c r="L12" t="s">
-        <v>153</v>
-      </c>
-      <c r="M12" s="31">
-        <v>1.8700000000000001E-5</v>
-      </c>
-      <c r="N12" s="31">
-        <v>1.2099999999999999E-5</v>
-      </c>
-      <c r="O12" s="34">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="P12" s="31">
-        <v>3.2399999999999999E-6</v>
-      </c>
-      <c r="Q12" s="31">
-        <v>3.2399999999999999E-6</v>
-      </c>
-      <c r="R12" s="31">
-        <v>6.0000000000000002E-6</v>
-      </c>
-      <c r="S12" s="34">
-        <v>1.4800000000000001E-5</v>
-      </c>
-      <c r="T12" s="31">
-        <v>3.0299999999999998E-6</v>
-      </c>
-      <c r="U12" s="31">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="V12" s="31">
-        <v>1.38E-5</v>
+      <c r="L12" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="M12" s="57">
+        <v>18.7</v>
+      </c>
+      <c r="N12" s="57">
+        <v>12.1</v>
+      </c>
+      <c r="O12" s="57">
+        <v>2</v>
+      </c>
+      <c r="P12" s="57">
+        <v>3.2399999999999998</v>
+      </c>
+      <c r="Q12" s="57">
+        <v>3.2399999999999998</v>
+      </c>
+      <c r="R12" s="57">
+        <v>6</v>
+      </c>
+      <c r="S12" s="57">
+        <v>14.8</v>
+      </c>
+      <c r="T12" s="57">
+        <v>3.03</v>
+      </c>
+      <c r="U12" s="57">
+        <v>2</v>
+      </c>
+      <c r="V12" s="58">
+        <v>13.8</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -3084,95 +3360,95 @@
         <v>3.3050000000000001E-4</v>
       </c>
       <c r="G13" s="32"/>
-      <c r="L13" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="M13" s="33">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="N13" s="33">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="O13" s="33">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="P13" s="33">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="Q13" s="33">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="R13" s="33">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="S13" s="33">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="T13" s="33">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="U13" s="33">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="V13" s="33">
-        <v>9.9999999999999995E-7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="L14" t="s">
-        <v>155</v>
-      </c>
-      <c r="M14" s="31">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="N14" s="31">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="O14" s="31">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="P14" s="31">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="Q14" s="31">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="R14" s="31">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="S14" s="31">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="T14" s="31">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="U14" s="31">
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="V14" s="31">
-        <v>9.9999999999999995E-7</v>
+      <c r="L13" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="M13" s="59">
+        <v>2</v>
+      </c>
+      <c r="N13" s="59">
+        <v>1</v>
+      </c>
+      <c r="O13" s="59">
+        <v>2</v>
+      </c>
+      <c r="P13" s="59">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="59">
+        <v>1</v>
+      </c>
+      <c r="R13" s="59">
+        <v>2</v>
+      </c>
+      <c r="S13" s="59">
+        <v>1</v>
+      </c>
+      <c r="T13" s="59">
+        <v>1</v>
+      </c>
+      <c r="U13" s="59">
+        <v>2</v>
+      </c>
+      <c r="V13" s="60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L14" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="M14" s="57">
+        <v>3</v>
+      </c>
+      <c r="N14" s="57">
+        <v>1</v>
+      </c>
+      <c r="O14" s="57">
+        <v>1</v>
+      </c>
+      <c r="P14" s="57">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="57">
+        <v>1</v>
+      </c>
+      <c r="R14" s="57">
+        <v>2</v>
+      </c>
+      <c r="S14" s="57">
+        <v>1</v>
+      </c>
+      <c r="T14" s="57">
+        <v>1</v>
+      </c>
+      <c r="U14" s="57">
+        <v>2</v>
+      </c>
+      <c r="V14" s="58">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
+        <v>134</v>
+      </c>
+      <c r="F16" t="s">
         <v>135</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>136</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>137</v>
       </c>
-      <c r="H16" t="s">
-        <v>138</v>
-      </c>
       <c r="I16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D17" s="32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E17" s="33">
         <v>1.8000000000000001E-4</v>
@@ -3193,7 +3469,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D18" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E18" s="33">
         <f>E17/I17</f>
@@ -3214,7 +3490,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E19">
         <v>0.55000000000000004</v>
@@ -3231,7 +3507,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E20" s="31">
         <f>F2*E19</f>
@@ -3252,7 +3528,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E21" s="31">
         <v>1.34E-4</v>
@@ -3269,28 +3545,28 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E22" s="31">
         <f>(E21-E17)/E17</f>
         <v>-0.25555555555555559</v>
       </c>
       <c r="F22" s="31">
-        <f t="shared" ref="F22:H22" si="1">(F21-F17)/F17</f>
+        <f t="shared" ref="F22:H22" si="3">(F21-F17)/F17</f>
         <v>-4.7058823529411715E-2</v>
       </c>
       <c r="G22" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.57866666666666688</v>
       </c>
       <c r="H22" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-0.52</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D23" s="32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E23" s="32">
         <v>74.941400000000002</v>
@@ -3311,7 +3587,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D24" s="32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E24">
         <f>POWER(10,E23/20)</f>
@@ -3332,7 +3608,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D25" s="32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E25" s="33">
         <v>200546600</v>
@@ -3348,17 +3624,17 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="D28" s="42" t="s">
-        <v>164</v>
+      <c r="D28" s="37" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -3376,22 +3652,22 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="41" t="s">
+      <c r="B31" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="C31" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="C31" s="41" t="s">
+      <c r="D31" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="D31" s="41" t="s">
+      <c r="E31" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="E31" s="41" t="s">
-        <v>138</v>
-      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
-        <v>140</v>
+      <c r="A32" s="35" t="s">
+        <v>139</v>
       </c>
       <c r="B32" s="33">
         <v>1.8000000000000001E-4</v>
@@ -3408,7 +3684,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B33">
         <v>0.55000000000000004</v>
@@ -3425,7 +3701,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B34" s="31">
         <v>1.34E-4</v>
@@ -3442,7 +3718,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B35" s="31">
         <v>-0.25600000000000001</v>
@@ -3459,7 +3735,7 @@
     </row>
     <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="32" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C37" s="32" t="s">
         <v>46</v>
@@ -3474,21 +3750,21 @@
         <v>49</v>
       </c>
       <c r="G37" s="32" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="H37" s="32" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="I37" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="J37" s="43" t="s">
-        <v>173</v>
+        <v>164</v>
+      </c>
+      <c r="J37" s="38" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B38" s="31">
         <v>6.5499999999999998E-7</v>
@@ -3521,7 +3797,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="I39" s="31">
         <v>2.92E-4</v>
@@ -3532,7 +3808,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I40" s="31">
         <f>(I39-I38)/I38</f>
@@ -3545,7 +3821,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>